<commit_message>
feat: festival results prep
</commit_message>
<xml_diff>
--- a/scripts/open-players.xlsx
+++ b/scripts/open-players.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewwebb/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\develop\presentation\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{93866034-EC19-BD4A-9E00-71B54810681F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FEB00549-656D-4632-B1BE-AC4C05DEA92A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="500" windowWidth="23000" windowHeight="14380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="98">
   <si>
     <t>From the Tournament-Database of Chess-Results http://chess-results.com</t>
   </si>
@@ -28,7 +28,7 @@
     <t xml:space="preserve">Ilkley Chess Festival - Open </t>
   </si>
   <si>
-    <t>Last update 16.09.2022 00:09:22</t>
+    <t>Last update 18.09.2022 18:48:05</t>
   </si>
   <si>
     <t>Starting rank</t>
@@ -154,6 +154,12 @@
     <t>Wickens Tim</t>
   </si>
   <si>
+    <t>SCO</t>
+  </si>
+  <si>
+    <t>ISCO</t>
+  </si>
+  <si>
     <t>Edwards-Wright Miles D</t>
   </si>
   <si>
@@ -208,9 +214,6 @@
     <t>Ridge Michael</t>
   </si>
   <si>
-    <t>SCO</t>
-  </si>
-  <si>
     <t>Edinburgh</t>
   </si>
   <si>
@@ -289,12 +292,6 @@
     <t>Barrow</t>
   </si>
   <si>
-    <t>Corcoran Gary</t>
-  </si>
-  <si>
-    <t>Shipley</t>
-  </si>
-  <si>
     <t>Cuaresma Bien</t>
   </si>
   <si>
@@ -308,6 +305,9 @@
   </si>
   <si>
     <t>Purbeck</t>
+  </si>
+  <si>
+    <t>Cuaresma Gerald</t>
   </si>
   <si>
     <t>You find all details to this tournament under  http://chess-results.com/tnr665788.aspx?lan=1</t>
@@ -782,38 +782,38 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
     <col min="2" max="2" width="0" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" customWidth="1"/>
-    <col min="5" max="5" width="4.1640625" customWidth="1"/>
-    <col min="6" max="6" width="4.6640625" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="5" max="5" width="4.140625" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>4</v>
       </c>
@@ -834,7 +834,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>1</v>
       </c>
@@ -855,7 +855,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>2</v>
       </c>
@@ -876,7 +876,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>3</v>
       </c>
@@ -897,7 +897,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>4</v>
       </c>
@@ -918,7 +918,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>5</v>
       </c>
@@ -939,7 +939,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>6</v>
       </c>
@@ -960,7 +960,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>7</v>
       </c>
@@ -981,7 +981,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>8</v>
       </c>
@@ -1002,7 +1002,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>9</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>10</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>11</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>12</v>
       </c>
@@ -1086,7 +1086,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>13</v>
       </c>
@@ -1107,7 +1107,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>14</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>15</v>
       </c>
@@ -1149,7 +1149,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>16</v>
       </c>
@@ -1170,7 +1170,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>17</v>
       </c>
@@ -1180,20 +1180,22 @@
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="5" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="F22" s="7">
         <v>2035</v>
       </c>
-      <c r="G22" s="5"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G22" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>18</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D23" s="7">
         <v>424072</v>
@@ -1205,16 +1207,16 @@
         <v>2034</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>19</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D24" s="7">
         <v>499927</v>
@@ -1226,16 +1228,16 @@
         <v>2033</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>20</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D25" s="7">
         <v>462942</v>
@@ -1247,16 +1249,16 @@
         <v>2031</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>21</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D26" s="7">
         <v>417041</v>
@@ -1268,16 +1270,16 @@
         <v>2028</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>22</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="5" t="s">
@@ -1287,16 +1289,16 @@
         <v>2026</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>23</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D28" s="7">
         <v>461962</v>
@@ -1308,16 +1310,16 @@
         <v>2026</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>24</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D29" s="7">
         <v>405213</v>
@@ -1329,58 +1331,58 @@
         <v>2022</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>25</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D30" s="7">
         <v>410942</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F30" s="7">
         <v>2015</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>26</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D31" s="7">
         <v>2401894</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="F31" s="7">
         <v>2010</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>27</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D32" s="7">
         <v>435880</v>
@@ -1392,16 +1394,16 @@
         <v>2009</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>28</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D33" s="7">
         <v>8601330</v>
@@ -1416,13 +1418,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>29</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D34" s="7">
         <v>412600</v>
@@ -1434,16 +1436,16 @@
         <v>2005</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>30</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D35" s="7">
         <v>424226</v>
@@ -1455,16 +1457,16 @@
         <v>2001</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>31</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D36" s="7">
         <v>458651</v>
@@ -1476,16 +1478,16 @@
         <v>2000</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>32</v>
       </c>
       <c r="B37" s="5"/>
       <c r="C37" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D37" s="7">
         <v>423947</v>
@@ -1500,13 +1502,13 @@
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>33</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D38" s="7">
         <v>343113833</v>
@@ -1518,16 +1520,16 @@
         <v>1968</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>34</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D39" s="7">
         <v>422240</v>
@@ -1539,16 +1541,16 @@
         <v>1955</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>35</v>
       </c>
       <c r="B40" s="5"/>
       <c r="C40" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D40" s="7">
         <v>469084</v>
@@ -1560,16 +1562,16 @@
         <v>1952</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>36</v>
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D41" s="7">
         <v>424560</v>
@@ -1581,16 +1583,16 @@
         <v>1921</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>37</v>
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D42" s="7">
         <v>418803</v>
@@ -1602,16 +1604,16 @@
         <v>1877</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>38</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D43" s="7">
         <v>438588</v>
@@ -1623,16 +1625,16 @@
         <v>1854</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>39</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D44" s="7">
         <v>468517</v>
@@ -1644,16 +1646,16 @@
         <v>1831</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>40</v>
       </c>
       <c r="B45" s="5"/>
       <c r="C45" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D45" s="7">
         <v>413828</v>
@@ -1668,13 +1670,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>41</v>
       </c>
       <c r="B46" s="5"/>
       <c r="C46" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D46" s="7">
         <v>451827</v>
@@ -1686,31 +1688,31 @@
         <v>1811</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>42</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D47" s="7">
-        <v>418560</v>
+        <v>451681</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F47" s="7">
-        <v>1806</v>
+        <v>1710</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>43</v>
       </c>
@@ -1719,64 +1721,64 @@
         <v>91</v>
       </c>
       <c r="D48" s="7">
-        <v>451681</v>
+        <v>484253</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F48" s="7">
-        <v>1710</v>
+        <v>1677</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <v>44</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D49" s="7">
-        <v>484253</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="D49" s="7"/>
       <c r="E49" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F49" s="7">
-        <v>1677</v>
+        <v>1255</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="6">
         <v>45</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D50" s="7"/>
+        <v>95</v>
+      </c>
+      <c r="D50" s="7">
+        <v>499935</v>
+      </c>
       <c r="E50" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F50" s="7">
-        <v>1255</v>
+        <v>1980</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>97</v>
       </c>
@@ -1789,7 +1791,7 @@
   </hyperlinks>
   <pageMargins left="0.5" right="0.3" top="0.4" bottom="0.7" header="0" footer="0.2"/>
   <headerFooter>
-    <oddFooter>&amp;L&amp;9Chess-Tournament-Results-Server: Chess-Results.com&amp;C&amp;9          Page &amp;P / &amp;N&amp;R&amp;9created on 16.09.2022 00:25:04</oddFooter>
+    <oddFooter>&amp;L&amp;9Chess-Tournament-Results-Server: Chess-Results.com&amp;C&amp;9          Page &amp;P / &amp;N&amp;R&amp;9created on 13.10.2022 17:46:47</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>